<commit_message>
Users can now publish in FB
</commit_message>
<xml_diff>
--- a/Meta2/sd_checklist_meta2.xlsx
+++ b/Meta2/sd_checklist_meta2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidadedecoimbra154-my.sharepoint.com/personal/uc2018288464_student_uc_pt/Documents/Univerisdade/UNI-Meu/PL SD/Projeto/SDProject/Meta2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{F1CE4857-0108-4B19-986A-8BE74ACAC475}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7BD82BD-CE32-4D0C-AB88-0FD81C43A265}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{F1CE4857-0108-4B19-986A-8BE74ACAC475}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA2EB79A-55CD-41B2-BBB8-3ED4E9BBE441}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22296" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020-21" sheetId="3" r:id="rId1"/>
@@ -796,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BR47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="86" zoomScaleNormal="121" zoomScalePageLayoutView="121" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="86" zoomScaleNormal="121" zoomScalePageLayoutView="121" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="13.8"/>
@@ -840,7 +840,7 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" ref="C5:AH5" si="0">C6+C21+C25+C31+C36+C41</f>
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="0"/>
@@ -2171,6 +2171,9 @@
       <c r="B28" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A29" s="3">
@@ -2178,6 +2181,9 @@
       </c>
       <c r="B29" s="4" t="s">
         <v>38</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:70" s="3" customFormat="1" ht="18">
@@ -2201,7 +2207,7 @@
       </c>
       <c r="C31" s="1">
         <f t="shared" ref="C31:AH31" si="9">SUM(C32:C35)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" si="9"/>
@@ -2479,6 +2485,9 @@
       <c r="B32" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="C32" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A33" s="3">
@@ -2487,6 +2496,9 @@
       <c r="B33" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="C33" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A34" s="3">
@@ -2495,6 +2507,9 @@
       <c r="B34" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="C34" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="35" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="A35" s="3">
@@ -2503,6 +2518,9 @@
       <c r="B35" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="C35" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="36" spans="1:70" s="1" customFormat="1" ht="18">
       <c r="B36" s="2" t="s">
@@ -2790,6 +2808,7 @@
       <c r="B38" s="4" t="s">
         <v>46</v>
       </c>
+      <c r="C38" s="8"/>
     </row>
     <row r="39" spans="1:70" s="3" customFormat="1" ht="18">
       <c r="B39" s="4" t="s">

</xml_diff>